<commit_message>
finish PA voting data
</commit_message>
<xml_diff>
--- a/data/cleaned/voting/PA-scorecard-2015.xlsx
+++ b/data/cleaned/voting/PA-scorecard-2015.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dan/working/enviro_papers/data/cleaned/voting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DB5CF8-E804-7842-902F-C04EC85FD393}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EC8D0C-13CA-674B-BCA5-8E1A570D9C4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="House" sheetId="1" r:id="rId1"/>
@@ -1003,178 +1003,167 @@
     <t>Delaying Action on Climate Change</t>
   </si>
   <si>
-    <t>Alloway, Richard</t>
-  </si>
-  <si>
-    <t>Argall, David</t>
-  </si>
-  <si>
-    <t>Aument, Ryan</t>
-  </si>
-  <si>
-    <t>Baker, Lisa</t>
-  </si>
-  <si>
-    <t>Bartolotta, Camera</t>
-  </si>
-  <si>
-    <t>Blake, John</t>
-  </si>
-  <si>
-    <t>Boscola, Lisa</t>
-  </si>
-  <si>
-    <t>Brewster, James</t>
-  </si>
-  <si>
-    <t>Brooks, Michele</t>
-  </si>
-  <si>
-    <t>Browne, Patrick</t>
-  </si>
-  <si>
-    <t>Corman, Jake</t>
-  </si>
-  <si>
-    <t>Costa, Jay</t>
-  </si>
-  <si>
-    <t>Dinniman, Andrew</t>
-  </si>
-  <si>
-    <t>Eichelberger, John</t>
-  </si>
-  <si>
-    <t>Farnese, Lawrence</t>
-  </si>
-  <si>
-    <t>Folmer, Mike</t>
-  </si>
-  <si>
-    <t>Fontana, Wayne</t>
-  </si>
-  <si>
-    <t>Gordner, John</t>
-  </si>
-  <si>
-    <t>Greenleaf, Stewart</t>
-  </si>
-  <si>
-    <t>Haywood, Art</t>
-  </si>
-  <si>
-    <t>Hughes, Vincent</t>
-  </si>
-  <si>
-    <t>Hutchinson, Scott</t>
-  </si>
-  <si>
-    <r>
-      <t>Killion, Thomas</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>†</t>
-    </r>
-  </si>
-  <si>
-    <t>Kitchen, Shirley</t>
-  </si>
-  <si>
-    <t>Leach, Daylin</t>
-  </si>
-  <si>
-    <t>McGarrigle, Thomas</t>
-  </si>
-  <si>
-    <t>McIlhinney, Charles</t>
-  </si>
-  <si>
-    <t>Mensch, Bob</t>
-  </si>
-  <si>
-    <t>Rafferty, John</t>
-  </si>
-  <si>
-    <t>Reschenthaler, Guy</t>
-  </si>
-  <si>
-    <t>Sabatina, John</t>
-  </si>
-  <si>
-    <t>Scarnati, Joseph</t>
-  </si>
-  <si>
     <t>PA</t>
   </si>
   <si>
     <t>Senate</t>
   </si>
   <si>
-    <t>Scavello, Mario</t>
-  </si>
-  <si>
-    <t>Schwank, Judith</t>
-  </si>
-  <si>
-    <t>Smucker, Lloyd</t>
-  </si>
-  <si>
-    <t>Stefano, Patrick</t>
-  </si>
-  <si>
-    <t>Tartaglione, Christine</t>
-  </si>
-  <si>
-    <t>Teplitz, Rob</t>
-  </si>
-  <si>
-    <t>Tomlinson, Robert</t>
-  </si>
-  <si>
-    <t>Vance, Patricia</t>
-  </si>
-  <si>
-    <t>Vogel, Elder</t>
-  </si>
-  <si>
-    <t>Vulakovich, Randy</t>
-  </si>
-  <si>
-    <t>Wagner, Scott</t>
-  </si>
-  <si>
-    <t>Ward, Kim</t>
-  </si>
-  <si>
-    <t>White, Donald</t>
-  </si>
-  <si>
-    <t>Wiley, Sean</t>
-  </si>
-  <si>
-    <t>Williams, Anthony</t>
-  </si>
-  <si>
-    <t>Wozniak, John</t>
-  </si>
-  <si>
-    <t>Yaw, Gene</t>
-  </si>
-  <si>
-    <t>Yudichak, John</t>
+    <t>Richard Alloway</t>
+  </si>
+  <si>
+    <t>David Argall</t>
+  </si>
+  <si>
+    <t>Ryan Aument</t>
+  </si>
+  <si>
+    <t>Lisa Baker</t>
+  </si>
+  <si>
+    <t>Camera Bartolotta</t>
+  </si>
+  <si>
+    <t>John Blake</t>
+  </si>
+  <si>
+    <t>Lisa Boscola</t>
+  </si>
+  <si>
+    <t>James Brewster</t>
+  </si>
+  <si>
+    <t>Michele Brooks</t>
+  </si>
+  <si>
+    <t>Patrick Browne</t>
+  </si>
+  <si>
+    <t>Jake Corman</t>
+  </si>
+  <si>
+    <t>Jay Costa</t>
+  </si>
+  <si>
+    <t>Andrew Dinniman</t>
+  </si>
+  <si>
+    <t>John Eichelberger</t>
+  </si>
+  <si>
+    <t>Lawrence Farnese</t>
+  </si>
+  <si>
+    <t>Mike Folmer</t>
+  </si>
+  <si>
+    <t>Wayne Fontana</t>
+  </si>
+  <si>
+    <t>John Gordner</t>
+  </si>
+  <si>
+    <t>Stewart Greenleaf</t>
+  </si>
+  <si>
+    <t>Art Haywood</t>
+  </si>
+  <si>
+    <t>Vincent Hughes</t>
+  </si>
+  <si>
+    <t>Scott Hutchinson</t>
+  </si>
+  <si>
+    <t>Thomas† Killion</t>
+  </si>
+  <si>
+    <t>Shirley Kitchen</t>
+  </si>
+  <si>
+    <t>Daylin Leach</t>
+  </si>
+  <si>
+    <t>Thomas McGarrigle</t>
+  </si>
+  <si>
+    <t>Charles McIlhinney</t>
+  </si>
+  <si>
+    <t>Bob Mensch</t>
+  </si>
+  <si>
+    <t>John Rafferty</t>
+  </si>
+  <si>
+    <t>Guy Reschenthaler</t>
+  </si>
+  <si>
+    <t>John Sabatina</t>
+  </si>
+  <si>
+    <t>Joseph Scarnati</t>
+  </si>
+  <si>
+    <t>Mario Scavello</t>
+  </si>
+  <si>
+    <t>Judith Schwank</t>
+  </si>
+  <si>
+    <t>Lloyd Smucker</t>
+  </si>
+  <si>
+    <t>Patrick Stefano</t>
+  </si>
+  <si>
+    <t>Christine Tartaglione</t>
+  </si>
+  <si>
+    <t>Rob Teplitz</t>
+  </si>
+  <si>
+    <t>Robert Tomlinson</t>
+  </si>
+  <si>
+    <t>Patricia Vance</t>
+  </si>
+  <si>
+    <t>Elder Vogel</t>
+  </si>
+  <si>
+    <t>Randy Vulakovich</t>
+  </si>
+  <si>
+    <t>Scott Wagner</t>
+  </si>
+  <si>
+    <t>Kim Ward</t>
+  </si>
+  <si>
+    <t>Donald White</t>
+  </si>
+  <si>
+    <t>Sean Wiley</t>
+  </si>
+  <si>
+    <t>Anthony Williams</t>
+  </si>
+  <si>
+    <t>John Wozniak</t>
+  </si>
+  <si>
+    <t>Gene Yaw</t>
+  </si>
+  <si>
+    <t>John Yudichak</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1182,12 +1171,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1220,828 +1203,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="82">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2377,7 +1539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -13766,8 +12928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13819,16 +12981,16 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B2">
         <v>2015</v>
       </c>
       <c r="C2" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D2" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -13857,16 +13019,16 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B3">
         <v>2015</v>
       </c>
       <c r="C3" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D3" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -13895,16 +13057,16 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B4">
         <v>2015</v>
       </c>
       <c r="C4" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D4" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
@@ -13933,16 +13095,16 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B5">
         <v>2015</v>
       </c>
       <c r="C5" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D5" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
@@ -13971,16 +13133,16 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B6">
         <v>2015</v>
       </c>
       <c r="C6" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D6" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
@@ -14009,16 +13171,16 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B7">
         <v>2015</v>
       </c>
       <c r="C7" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D7" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
@@ -14047,16 +13209,16 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B8">
         <v>2015</v>
       </c>
       <c r="C8" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D8" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E8" t="s">
         <v>1</v>
@@ -14085,16 +13247,16 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B9">
         <v>2015</v>
       </c>
       <c r="C9" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D9" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
@@ -14123,16 +13285,16 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B10">
         <v>2015</v>
       </c>
       <c r="C10" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D10" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
@@ -14161,16 +13323,16 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B11">
         <v>2015</v>
       </c>
       <c r="C11" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D11" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E11" t="s">
         <v>2</v>
@@ -14199,16 +13361,16 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B12">
         <v>2015</v>
       </c>
       <c r="C12" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D12" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="E12" t="s">
         <v>2</v>
@@ -14237,16 +13399,16 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B13">
         <v>2015</v>
       </c>
       <c r="C13" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D13" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E13" t="s">
         <v>1</v>
@@ -14275,16 +13437,16 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B14">
         <v>2015</v>
       </c>
       <c r="C14" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D14" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E14" t="s">
         <v>1</v>
@@ -14313,16 +13475,16 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B15">
         <v>2015</v>
       </c>
       <c r="C15" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D15" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E15" t="s">
         <v>2</v>
@@ -14351,16 +13513,16 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B16">
         <v>2015</v>
       </c>
       <c r="C16" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D16" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="E16" t="s">
         <v>1</v>
@@ -14389,16 +13551,16 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B17">
         <v>2015</v>
       </c>
       <c r="C17" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D17" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="E17" t="s">
         <v>2</v>
@@ -14427,16 +13589,16 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B18">
         <v>2015</v>
       </c>
       <c r="C18" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D18" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="E18" t="s">
         <v>1</v>
@@ -14465,16 +13627,16 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B19">
         <v>2015</v>
       </c>
       <c r="C19" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D19" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="E19" t="s">
         <v>2</v>
@@ -14503,16 +13665,16 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B20">
         <v>2015</v>
       </c>
       <c r="C20" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D20" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="E20" t="s">
         <v>2</v>
@@ -14541,16 +13703,16 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B21">
         <v>2015</v>
       </c>
       <c r="C21" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D21" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
@@ -14579,16 +13741,16 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B22">
         <v>2015</v>
       </c>
       <c r="C22" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D22" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
@@ -14617,16 +13779,16 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B23">
         <v>2015</v>
       </c>
       <c r="C23" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D23" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="E23" t="s">
         <v>2</v>
@@ -14653,18 +13815,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B24">
         <v>2015</v>
       </c>
       <c r="C24" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D24" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E24" t="s">
         <v>2</v>
@@ -14693,16 +13855,16 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B25">
         <v>2015</v>
       </c>
       <c r="C25" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D25" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="E25" t="s">
         <v>1</v>
@@ -14731,16 +13893,16 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B26">
         <v>2015</v>
       </c>
       <c r="C26" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D26" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E26" t="s">
         <v>1</v>
@@ -14769,16 +13931,16 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B27">
         <v>2015</v>
       </c>
       <c r="C27" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D27" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E27" t="s">
         <v>2</v>
@@ -14807,16 +13969,16 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B28">
         <v>2015</v>
       </c>
       <c r="C28" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D28" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="E28" t="s">
         <v>2</v>
@@ -14845,16 +14007,16 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B29">
         <v>2015</v>
       </c>
       <c r="C29" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D29" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E29" t="s">
         <v>2</v>
@@ -14883,16 +14045,16 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B30">
         <v>2015</v>
       </c>
       <c r="C30" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D30" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="E30" t="s">
         <v>2</v>
@@ -14921,16 +14083,16 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B31">
         <v>2015</v>
       </c>
       <c r="C31" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D31" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E31" t="s">
         <v>2</v>
@@ -14959,16 +14121,16 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
+        <v>326</v>
+      </c>
+      <c r="B32">
+        <v>2015</v>
+      </c>
+      <c r="C32" t="s">
+        <v>327</v>
+      </c>
+      <c r="D32" t="s">
         <v>358</v>
-      </c>
-      <c r="B32">
-        <v>2015</v>
-      </c>
-      <c r="C32" t="s">
-        <v>359</v>
-      </c>
-      <c r="D32" t="s">
-        <v>356</v>
       </c>
       <c r="E32" t="s">
         <v>1</v>
@@ -14997,16 +14159,16 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B33">
         <v>2015</v>
       </c>
       <c r="C33" t="s">
+        <v>327</v>
+      </c>
+      <c r="D33" t="s">
         <v>359</v>
-      </c>
-      <c r="D33" t="s">
-        <v>357</v>
       </c>
       <c r="E33" t="s">
         <v>2</v>
@@ -15035,13 +14197,13 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B34">
         <v>2015</v>
       </c>
       <c r="C34" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D34" t="s">
         <v>360</v>
@@ -15073,13 +14235,13 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B35">
         <v>2015</v>
       </c>
       <c r="C35" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D35" t="s">
         <v>361</v>
@@ -15111,13 +14273,13 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B36">
         <v>2015</v>
       </c>
       <c r="C36" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D36" t="s">
         <v>362</v>
@@ -15149,13 +14311,13 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B37">
         <v>2015</v>
       </c>
       <c r="C37" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D37" t="s">
         <v>363</v>
@@ -15187,13 +14349,13 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B38">
         <v>2015</v>
       </c>
       <c r="C38" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D38" t="s">
         <v>364</v>
@@ -15225,13 +14387,13 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B39">
         <v>2015</v>
       </c>
       <c r="C39" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D39" t="s">
         <v>365</v>
@@ -15263,13 +14425,13 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B40">
         <v>2015</v>
       </c>
       <c r="C40" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D40" t="s">
         <v>366</v>
@@ -15301,13 +14463,13 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B41">
         <v>2015</v>
       </c>
       <c r="C41" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D41" t="s">
         <v>367</v>
@@ -15339,13 +14501,13 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B42">
         <v>2015</v>
       </c>
       <c r="C42" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D42" t="s">
         <v>368</v>
@@ -15377,13 +14539,13 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B43">
         <v>2015</v>
       </c>
       <c r="C43" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D43" t="s">
         <v>369</v>
@@ -15415,13 +14577,13 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B44">
         <v>2015</v>
       </c>
       <c r="C44" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D44" t="s">
         <v>370</v>
@@ -15453,13 +14615,13 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B45">
         <v>2015</v>
       </c>
       <c r="C45" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D45" t="s">
         <v>371</v>
@@ -15491,13 +14653,13 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B46">
         <v>2015</v>
       </c>
       <c r="C46" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D46" t="s">
         <v>372</v>
@@ -15529,13 +14691,13 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B47">
         <v>2015</v>
       </c>
       <c r="C47" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D47" t="s">
         <v>373</v>
@@ -15567,13 +14729,13 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B48">
         <v>2015</v>
       </c>
       <c r="C48" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D48" t="s">
         <v>374</v>
@@ -15605,13 +14767,13 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B49">
         <v>2015</v>
       </c>
       <c r="C49" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D49" t="s">
         <v>375</v>
@@ -15643,13 +14805,13 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B50">
         <v>2015</v>
       </c>
       <c r="C50" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D50" t="s">
         <v>376</v>
@@ -15681,13 +14843,13 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="B51">
         <v>2015</v>
       </c>
       <c r="C51" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="D51" t="s">
         <v>377</v>

</xml_diff>